<commit_message>
Updating the entire EMDAT & IFRC databases to match with PostGIS-requirements, to update taxonomies and correct for errors found in the process
</commit_message>
<xml_diff>
--- a/Taxonomies/Monty_DataSources.xlsx
+++ b/Taxonomies/Monty_DataSources.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="118">
   <si>
     <t xml:space="preserve">src_db_code</t>
   </si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">custodian</t>
   </si>
   <si>
-    <t xml:space="preserve">Apache-2-like</t>
+    <t xml:space="preserve">CC BY</t>
   </si>
   <si>
     <t xml:space="preserve">UNO_damass</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">https://unosat.org/products/</t>
   </si>
   <si>
-    <t xml:space="preserve">CCA</t>
+    <t xml:space="preserve">CC BY-SA</t>
   </si>
   <si>
     <t xml:space="preserve">COP_damass</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">https://emergency.copernicus.eu/</t>
   </si>
   <si>
-    <t xml:space="preserve">GO-App</t>
+    <t xml:space="preserve">GO-EA</t>
   </si>
   <si>
     <t xml:space="preserve">IFRC Emergency Appeals (EA)</t>
@@ -256,48 +256,54 @@
     <t xml:space="preserve">www.internal-displacement.org</t>
   </si>
   <si>
+    <t xml:space="preserve">CC BY-IGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDACS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Disaster Alert and Coordination System (GDACS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EC-JRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European Commission - Joint Research Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coordination@gdacs.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.gdacs.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mediator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIT License</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLobal IDEntifier numbers (GLIDE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asian Disaster Reduction Center (ADRC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gliderep@adrc.asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://glidenumber.net</t>
+  </si>
+  <si>
     <t xml:space="preserve">unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">GDACS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global Disaster Alert and Coordination System (GDACS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EC-JRC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">European Commission - Joint Research Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coordination@gdacs.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.gdacs.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mediator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLIDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLobal IDEntifier numbers (GLIDE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADRC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asian Disaster Reduction Center (ADRC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gliderep@adrc.asia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://glidenumber.net</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO-Maps</t>
   </si>
   <si>
@@ -307,10 +313,10 @@
     <t xml:space="preserve">https://go-user-library.ifrc.org/maps</t>
   </si>
   <si>
-    <t xml:space="preserve">Shakemaps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Earthquake Catalog</t>
+    <t xml:space="preserve">Atlas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atlas Earthquake ShakeMap Catalog</t>
   </si>
   <si>
     <t xml:space="preserve">USGS</t>
@@ -325,7 +331,49 @@
     <t xml:space="preserve">https://www.usgs.gov/survey-manual/11006-use-copyrighted-material-usgs-information-products</t>
   </si>
   <si>
-    <t xml:space="preserve">U.S Public Domain</t>
+    <t xml:space="preserve">GAUL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Administrative Unit Layers (GAUL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food and Agriculture Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fao-data@fao.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://data.apps.fao.org/map/catalog/static/search?keyword=HiH_boundaries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GovDes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Official Government or UN ADM Boundaries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dartmouth Flood Observatory (DFO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniColumbia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University of Columbia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kettner@colorado.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://floodobservatory.colorado.edu/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCA 4.0 BY</t>
   </si>
 </sst>
 </file>
@@ -335,11 +383,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -361,12 +410,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -411,7 +469,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -426,6 +484,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -445,10 +511,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ18"/>
+  <dimension ref="A1:AMJ21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8:K8"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -522,6 +588,8 @@
       <c r="J2" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
@@ -556,6 +624,8 @@
       <c r="J3" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
@@ -619,7 +689,7 @@
       <c r="I5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="0" t="s">
         <v>39</v>
       </c>
     </row>
@@ -783,6 +853,8 @@
       <c r="J10" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -941,21 +1013,21 @@
         <v>85</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>44</v>
@@ -964,24 +1036,24 @@
         <v>45</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>29</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>50</v>
@@ -999,7 +1071,7 @@
         <v>54</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>29</v>
@@ -1010,16 +1082,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>25</v>
@@ -1028,16 +1100,112 @@
         <v>26</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>29</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>101</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>